<commit_message>
Updated list of books
</commit_message>
<xml_diff>
--- a/assets/datasource/books.xlsx
+++ b/assets/datasource/books.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\VisualStudio\BookshopVue\BookshopVue\assets\datasource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C975C6F-3904-4CE7-808F-501420329983}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF11F4E2-2A06-43F1-A891-65BFA828D4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>Title</t>
   </si>
@@ -223,6 +223,15 @@
   </si>
   <si>
     <t>Raven Leilani</t>
+  </si>
+  <si>
+    <t>Mayflies</t>
+  </si>
+  <si>
+    <t>Andrew O'Hagan</t>
+  </si>
+  <si>
+    <t>Later</t>
   </si>
 </sst>
 </file>
@@ -549,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,6 +935,34 @@
         <v>8.99</v>
       </c>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28">
+        <v>8.99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>